<commit_message>
try upload 3 again
</commit_message>
<xml_diff>
--- a/dataAnalysis/spreadsheets/MeasurementsCorrelation.xlsx
+++ b/dataAnalysis/spreadsheets/MeasurementsCorrelation.xlsx
@@ -25,7 +25,7 @@
     <t>Leptin</t>
   </si>
   <si>
-    <t>Weight</t>
+    <t>BMI</t>
   </si>
   <si>
     <t>Calories</t>
@@ -112,8 +112,8 @@
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="true"/>
     <col min="2" max="2" width="14.7109375" customWidth="true"/>
-    <col min="3" max="3" width="14.7109375" customWidth="true"/>
-    <col min="4" max="4" width="14.7109375" customWidth="true"/>
+    <col min="3" max="3" width="15.7109375" customWidth="true"/>
+    <col min="4" max="4" width="15.7109375" customWidth="true"/>
     <col min="5" max="5" width="13.7109375" customWidth="true"/>
   </cols>
   <sheetData>
@@ -142,13 +142,13 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>-0.044923655142946384</v>
+        <v>-0.046295178066277004</v>
       </c>
       <c r="D2">
-        <v>-0.36883644379347591</v>
+        <v>-0.4814930477872299</v>
       </c>
       <c r="E2">
-        <v>0.055599594410958922</v>
+        <v>-0.25485144331159998</v>
       </c>
     </row>
     <row r="3">
@@ -156,16 +156,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>-0.044923655142946384</v>
+        <v>-0.046295178066277004</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>-0.033564798650924488</v>
+        <v>-0.006878549834324503</v>
       </c>
       <c r="E3">
-        <v>0.1550867260536285</v>
+        <v>0.013940261464136558</v>
       </c>
     </row>
     <row r="4">
@@ -173,16 +173,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>-0.36883644379347591</v>
+        <v>-0.4814930477872299</v>
       </c>
       <c r="C4">
-        <v>-0.033564798650924488</v>
+        <v>-0.006878549834324503</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.031924028395671357</v>
+        <v>-0.25619521300354525</v>
       </c>
     </row>
     <row r="5">
@@ -190,13 +190,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.055599594410958922</v>
+        <v>-0.25485144331159998</v>
       </c>
       <c r="C5">
-        <v>0.1550867260536285</v>
+        <v>0.013940261464136558</v>
       </c>
       <c r="D5">
-        <v>0.031924028395671357</v>
+        <v>-0.25619521300354525</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -212,9 +212,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.7109375" customWidth="true"/>
-    <col min="2" max="2" width="14.7109375" customWidth="true"/>
-    <col min="3" max="3" width="12.7109375" customWidth="true"/>
-    <col min="4" max="4" width="14.7109375" customWidth="true"/>
+    <col min="2" max="2" width="13.7109375" customWidth="true"/>
+    <col min="3" max="3" width="11.7109375" customWidth="true"/>
+    <col min="4" max="4" width="13.7109375" customWidth="true"/>
     <col min="5" max="5" width="12.7109375" customWidth="true"/>
   </cols>
   <sheetData>
@@ -243,13 +243,13 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.7058810366732795</v>
+        <v>0.85995285403144428</v>
       </c>
       <c r="D2">
-        <v>0.0013228926812628714</v>
+        <v>0.050356403552665012</v>
       </c>
       <c r="E2">
-        <v>0.64035273477120036</v>
+        <v>0.3235592506313606</v>
       </c>
     </row>
     <row r="3">
@@ -257,16 +257,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.7058810366732795</v>
+        <v>0.85995285403144428</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0.77801446054743151</v>
+        <v>0.97909716700286242</v>
       </c>
       <c r="E3">
-        <v>0.19015049884239266</v>
+        <v>0.95765122396067226</v>
       </c>
     </row>
     <row r="4">
@@ -274,16 +274,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.0013228926812628714</v>
+        <v>0.050356403552665012</v>
       </c>
       <c r="C4">
-        <v>0.77801446054743151</v>
+        <v>0.97909716700286242</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0.78860727146603693</v>
+        <v>0.32092613009253734</v>
       </c>
     </row>
     <row r="5">
@@ -291,13 +291,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.64035273477120036</v>
+        <v>0.3235592506313606</v>
       </c>
       <c r="C5">
-        <v>0.19015049884239266</v>
+        <v>0.95765122396067226</v>
       </c>
       <c r="D5">
-        <v>0.78860727146603693</v>
+        <v>0.32092613009253734</v>
       </c>
       <c r="E5">
         <v>0</v>

</xml_diff>